<commit_message>
This is changes for whole project which working 6 TC for demo
</commit_message>
<xml_diff>
--- a/TuduApplication/TestData/Business configuration.xlsx
+++ b/TuduApplication/TestData/Business configuration.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Vikesh\Vikesh_eclipse\TuduApplication\TestData\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Vikesh\git\MYtudu\TuduApplication\TestData\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9FC64500-84D6-4AAB-B393-8F0B4D05B608}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6C263EF3-C8EA-4F12-8055-12A00DE16F77}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" activeTab="2" xr2:uid="{2966B0FB-1A44-4E56-B544-DAACB9056628}"/>
   </bookViews>

</xml_diff>

<commit_message>
Latest commit after demo
</commit_message>
<xml_diff>
--- a/TuduApplication/TestData/Business configuration.xlsx
+++ b/TuduApplication/TestData/Business configuration.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Vikesh\git\MYtudu\TuduApplication\TestData\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6C263EF3-C8EA-4F12-8055-12A00DE16F77}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FF7D69A1-0890-4389-8B2A-12E1DF250190}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" activeTab="2" xr2:uid="{2966B0FB-1A44-4E56-B544-DAACB9056628}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{2966B0FB-1A44-4E56-B544-DAACB9056628}"/>
   </bookViews>
   <sheets>
     <sheet name="SetUp" sheetId="2" r:id="rId1"/>
@@ -53,12 +53,6 @@
     <t>Password</t>
   </si>
   <si>
-    <t>salma.vakil@aimdek.com</t>
-  </si>
-  <si>
-    <t>Pass123$</t>
-  </si>
-  <si>
     <t>Browser selection</t>
   </si>
   <si>
@@ -72,6 +66,12 @@
   </si>
   <si>
     <t>http://abc.shopomate.com/#/login</t>
+  </si>
+  <si>
+    <t>Vikesh.patil@aimdek.com</t>
+  </si>
+  <si>
+    <t>Vikesh@1989</t>
   </si>
 </sst>
 </file>
@@ -433,15 +433,15 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{86130B3C-A02F-4A48-ABB8-B847A78180AE}">
-  <dimension ref="A1:B3"/>
+  <dimension ref="A1:B2"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection sqref="A1:B3"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A3" sqref="A3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="24" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="24.7109375" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="21.140625" customWidth="1"/>
   </cols>
   <sheetData>
@@ -455,18 +455,10 @@
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>5</v>
+        <v>10</v>
       </c>
       <c r="B2" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A3">
-        <v>112</v>
-      </c>
-      <c r="B3">
-        <v>336</v>
+        <v>11</v>
       </c>
     </row>
   </sheetData>
@@ -487,7 +479,7 @@
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="B1" s="2"/>
       <c r="C1" s="2"/>
@@ -505,13 +497,13 @@
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="B3" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="C3" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
     </row>
   </sheetData>
@@ -526,7 +518,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5DEBF86E-A04A-459C-A367-11770754C605}">
   <dimension ref="A1:A2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="A10" sqref="A10"/>
     </sheetView>
   </sheetViews>
@@ -537,12 +529,12 @@
   <sheetData>
     <row r="1" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
     </row>
     <row r="2" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
     </row>
   </sheetData>

</xml_diff>